<commit_message>
Added select style on left navigation drawer, fixed some worning
</commit_message>
<xml_diff>
--- a/data_reference/statistic_id232790_apple-iphone-smartphone-users-in-the-united-states-2012-2021.xlsx
+++ b/data_reference/statistic_id232790_apple-iphone-smartphone-users-in-the-united-states-2012-2021.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\SmartPhoneReact\data_reference\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8A75F0-A9FA-4EFA-80DF-0EF9AB3B6ADB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
+    <workbookView xWindow="2265" yWindow="3120" windowWidth="21600" windowHeight="14715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Statistic as Excel data file</t>
   </si>
@@ -123,24 +128,30 @@
     <t>2018</t>
   </si>
   <si>
-    <t>2019*</t>
-  </si>
-  <si>
     <t>2020*</t>
   </si>
   <si>
     <t>2021*</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="177" formatCode="#,##0"/>
-    <numFmt numFmtId="178" formatCode="#,##0.##"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.##"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -159,16 +170,21 @@
       <family val="2"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -183,139 +199,59 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
-      <protection/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
-      <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0"/>
-    <cellStyle name="Percent" xfId="15"/>
-    <cellStyle name="Currency" xfId="16"/>
-    <cellStyle name="Currency [0]" xfId="17"/>
-    <cellStyle name="Comma" xfId="18"/>
-    <cellStyle name="Comma [0]" xfId="19"/>
+  <cellStyles count="7">
+    <cellStyle name="Comma" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma [0]" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Currency" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Currency [0]" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Percent" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -638,38 +574,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.7142857142857" customWidth="1"/>
-    <col min="3" max="3" width="70.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="12.75">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" ht="12.75">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="12.75">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" ht="12.75">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="12.75">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
@@ -677,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="12.75">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
@@ -685,7 +621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="12.75">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
@@ -693,7 +629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="12.75">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -701,7 +637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="12.75">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -709,7 +645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="12.75">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
@@ -717,7 +653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="12.75">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
@@ -725,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="12.75">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
@@ -733,7 +669,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="12.75">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -741,12 +677,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" ht="12.75">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="12.75">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
@@ -754,7 +690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="12.75">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
@@ -762,7 +698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="12.75">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
@@ -770,7 +706,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="12.75">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
@@ -780,8 +716,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" location="Data!A1" display="Access data"/>
-    <hyperlink ref="C25" r:id="rId1" display="232790"/>
+    <hyperlink ref="B5" location="Data!A1" display="Access data" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C25" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -789,52 +725,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="B3:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B3:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="100.714285714286" customWidth="1"/>
-    <col min="3" max="3" width="5.85714285714286" customWidth="1"/>
+    <col min="2" max="2" width="100.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="12.75">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" ht="12.75">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="12.75">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="7">
-        <v>44.530000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="12.75">
+        <v>44.53</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="7">
-        <v>57.799999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="12.75">
+        <v>57.8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="7">
-        <v>72.299999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="12.75">
+        <v>72.3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
@@ -842,49 +788,49 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="12.75">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="7">
-        <v>90.099999999999994</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="12.75">
+        <v>90.1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="7">
-        <v>97.200000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="12.75">
+        <v>97.2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="7">
-        <v>101.90000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="12.75">
-      <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>101.9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="2">
+        <v>2019</v>
       </c>
       <c r="C13" s="7">
         <v>105.2</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="12.75">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="8">
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="12.75">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="7">
         <v>110.3</v>

</xml_diff>